<commit_message>
added average values to the test result tables
</commit_message>
<xml_diff>
--- a/Test Documents/Test 2 Results.xlsx
+++ b/Test Documents/Test 2 Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fibee\Desktop\Gamedev\Unity Projects\CMGT-Y2-T3-Advanced-Tools\Test Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33C9C43-ED51-4C1E-9DE5-AE77E27612E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5D282E-4080-4917-8ED0-7610DE2F73EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="4" xr2:uid="{34BB83C4-552E-4BC2-8E42-206248922780}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="9">
   <si>
     <t>[Frame]</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Cube</t>
+  </si>
+  <si>
+    <t>Sphere Average</t>
+  </si>
+  <si>
+    <t>MeshCube Average</t>
+  </si>
+  <si>
+    <t>Cube Average</t>
   </si>
 </sst>
 </file>
@@ -170,16 +179,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2269,7 +2278,7 @@
   <autoFilter ref="A1:C58" xr:uid="{ABCE5141-6159-4003-B27C-253CCB933C39}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E986D8EB-BACE-4784-AE7B-890E20583D8B}" uniqueName="1" name="[Frame]" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{51CB9CED-5DF1-46E2-B411-DD42EEA81A39}" uniqueName="2" name="-" queryTableFieldId="2" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{51CB9CED-5DF1-46E2-B411-DD42EEA81A39}" uniqueName="2" name="-" queryTableFieldId="2" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{0988D410-B79F-4834-96E8-0277690C78BE}" uniqueName="3" name="[FPS]" queryTableFieldId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2281,7 +2290,7 @@
   <autoFilter ref="A1:C68" xr:uid="{E75E4D72-F867-4224-871F-D157F03FB573}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C5330149-5F63-4B35-917D-49011453AABC}" uniqueName="1" name="[Frame]" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{7EF3454D-A310-4E8B-BA6C-1BF759047C3D}" uniqueName="2" name="-" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7EF3454D-A310-4E8B-BA6C-1BF759047C3D}" uniqueName="2" name="-" queryTableFieldId="2" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{0D9C52A4-8DAF-4165-93E9-3DB6BE58AC19}" uniqueName="3" name="[FPS]" queryTableFieldId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3856,7 +3865,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
@@ -3867,7 +3876,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
@@ -3878,7 +3887,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4">
@@ -3889,7 +3898,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5">
@@ -3900,7 +3909,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6">
@@ -3911,7 +3920,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7">
@@ -3922,7 +3931,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8">
@@ -3933,7 +3942,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9">
@@ -3944,7 +3953,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10">
@@ -3955,7 +3964,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="C11">
@@ -3966,7 +3975,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
       <c r="C12">
@@ -3977,7 +3986,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13">
@@ -3988,7 +3997,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14">
@@ -3999,7 +4008,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15">
@@ -4010,7 +4019,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="C16">
@@ -4021,7 +4030,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17">
@@ -4032,7 +4041,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="C18">
@@ -4043,7 +4052,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>1</v>
       </c>
       <c r="C19">
@@ -4054,7 +4063,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="C20">
@@ -4065,7 +4074,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" t="s">
         <v>1</v>
       </c>
       <c r="C21">
@@ -4076,7 +4085,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" t="s">
         <v>1</v>
       </c>
       <c r="C22">
@@ -4087,7 +4096,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23">
@@ -4098,7 +4107,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" t="s">
         <v>1</v>
       </c>
       <c r="C24">
@@ -4109,7 +4118,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25">
@@ -4120,7 +4129,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26">
@@ -4131,7 +4140,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" t="s">
         <v>1</v>
       </c>
       <c r="C27">
@@ -4142,7 +4151,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" t="s">
         <v>1</v>
       </c>
       <c r="C28">
@@ -4153,7 +4162,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29">
@@ -4164,7 +4173,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="C30">
@@ -4175,7 +4184,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31">
@@ -4186,7 +4195,7 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" t="s">
         <v>1</v>
       </c>
       <c r="C32">
@@ -4197,7 +4206,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" t="s">
         <v>1</v>
       </c>
       <c r="C33">
@@ -4208,7 +4217,7 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34">
@@ -4219,7 +4228,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" t="s">
         <v>1</v>
       </c>
       <c r="C35">
@@ -4230,7 +4239,7 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" t="s">
         <v>1</v>
       </c>
       <c r="C36">
@@ -4241,7 +4250,7 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37">
@@ -4252,7 +4261,7 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38">
@@ -4263,7 +4272,7 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="C39">
@@ -4274,7 +4283,7 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" t="s">
         <v>1</v>
       </c>
       <c r="C40">
@@ -4285,7 +4294,7 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" t="s">
         <v>1</v>
       </c>
       <c r="C41">
@@ -4296,7 +4305,7 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" t="s">
         <v>1</v>
       </c>
       <c r="C42">
@@ -4307,7 +4316,7 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" t="s">
         <v>1</v>
       </c>
       <c r="C43">
@@ -4318,7 +4327,7 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="C44">
@@ -4329,7 +4338,7 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" t="s">
         <v>1</v>
       </c>
       <c r="C45">
@@ -4340,7 +4349,7 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" t="s">
         <v>1</v>
       </c>
       <c r="C46">
@@ -4351,7 +4360,7 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" t="s">
         <v>1</v>
       </c>
       <c r="C47">
@@ -4362,7 +4371,7 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" t="s">
         <v>1</v>
       </c>
       <c r="C48">
@@ -4373,7 +4382,7 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" t="s">
         <v>1</v>
       </c>
       <c r="C49">
@@ -4384,7 +4393,7 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" t="s">
         <v>1</v>
       </c>
       <c r="C50">
@@ -4395,7 +4404,7 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" t="s">
         <v>1</v>
       </c>
       <c r="C51">
@@ -4406,7 +4415,7 @@
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" t="s">
         <v>1</v>
       </c>
       <c r="C52">
@@ -4417,7 +4426,7 @@
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" t="s">
         <v>1</v>
       </c>
       <c r="C53">
@@ -4428,7 +4437,7 @@
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" t="s">
         <v>1</v>
       </c>
       <c r="C54">
@@ -4439,7 +4448,7 @@
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" t="s">
         <v>1</v>
       </c>
       <c r="C55">
@@ -4450,7 +4459,7 @@
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" t="s">
         <v>1</v>
       </c>
       <c r="C56">
@@ -4461,7 +4470,7 @@
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" t="s">
         <v>1</v>
       </c>
       <c r="C57">
@@ -4472,7 +4481,7 @@
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" t="s">
         <v>1</v>
       </c>
       <c r="C58">
@@ -4517,7 +4526,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
@@ -4528,7 +4537,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
@@ -4539,7 +4548,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4">
@@ -4550,7 +4559,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5">
@@ -4561,7 +4570,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6">
@@ -4572,7 +4581,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7">
@@ -4583,7 +4592,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8">
@@ -4594,7 +4603,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9">
@@ -4605,7 +4614,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10">
@@ -4616,7 +4625,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="C11">
@@ -4627,7 +4636,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
       <c r="C12">
@@ -4638,7 +4647,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13">
@@ -4649,7 +4658,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14">
@@ -4660,7 +4669,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15">
@@ -4671,7 +4680,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="C16">
@@ -4682,7 +4691,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17">
@@ -4693,7 +4702,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="C18">
@@ -4704,7 +4713,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>1</v>
       </c>
       <c r="C19">
@@ -4715,7 +4724,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="C20">
@@ -4726,7 +4735,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" t="s">
         <v>1</v>
       </c>
       <c r="C21">
@@ -4737,7 +4746,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" t="s">
         <v>1</v>
       </c>
       <c r="C22">
@@ -4748,7 +4757,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23">
@@ -4759,7 +4768,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" t="s">
         <v>1</v>
       </c>
       <c r="C24">
@@ -4770,7 +4779,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25">
@@ -4781,7 +4790,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26">
@@ -4792,7 +4801,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" t="s">
         <v>1</v>
       </c>
       <c r="C27">
@@ -4803,7 +4812,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" t="s">
         <v>1</v>
       </c>
       <c r="C28">
@@ -4814,7 +4823,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29">
@@ -4825,7 +4834,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="C30">
@@ -4836,7 +4845,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31">
@@ -4847,7 +4856,7 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" t="s">
         <v>1</v>
       </c>
       <c r="C32">
@@ -4858,7 +4867,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" t="s">
         <v>1</v>
       </c>
       <c r="C33">
@@ -4869,7 +4878,7 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34">
@@ -4880,7 +4889,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" t="s">
         <v>1</v>
       </c>
       <c r="C35">
@@ -4891,7 +4900,7 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" t="s">
         <v>1</v>
       </c>
       <c r="C36">
@@ -4902,7 +4911,7 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37">
@@ -4913,7 +4922,7 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38">
@@ -4924,7 +4933,7 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="C39">
@@ -4935,7 +4944,7 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" t="s">
         <v>1</v>
       </c>
       <c r="C40">
@@ -4946,7 +4955,7 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" t="s">
         <v>1</v>
       </c>
       <c r="C41">
@@ -4957,7 +4966,7 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" t="s">
         <v>1</v>
       </c>
       <c r="C42">
@@ -4968,7 +4977,7 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" t="s">
         <v>1</v>
       </c>
       <c r="C43">
@@ -4979,7 +4988,7 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="C44">
@@ -4990,7 +4999,7 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" t="s">
         <v>1</v>
       </c>
       <c r="C45">
@@ -5001,7 +5010,7 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" t="s">
         <v>1</v>
       </c>
       <c r="C46">
@@ -5012,7 +5021,7 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" t="s">
         <v>1</v>
       </c>
       <c r="C47">
@@ -5023,7 +5032,7 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" t="s">
         <v>1</v>
       </c>
       <c r="C48">
@@ -5034,7 +5043,7 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" t="s">
         <v>1</v>
       </c>
       <c r="C49">
@@ -5045,7 +5054,7 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" t="s">
         <v>1</v>
       </c>
       <c r="C50">
@@ -5056,7 +5065,7 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" t="s">
         <v>1</v>
       </c>
       <c r="C51">
@@ -5067,7 +5076,7 @@
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" t="s">
         <v>1</v>
       </c>
       <c r="C52">
@@ -5078,7 +5087,7 @@
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" t="s">
         <v>1</v>
       </c>
       <c r="C53">
@@ -5089,7 +5098,7 @@
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" t="s">
         <v>1</v>
       </c>
       <c r="C54">
@@ -5100,7 +5109,7 @@
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" t="s">
         <v>1</v>
       </c>
       <c r="C55">
@@ -5111,7 +5120,7 @@
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" t="s">
         <v>1</v>
       </c>
       <c r="C56">
@@ -5122,7 +5131,7 @@
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" t="s">
         <v>1</v>
       </c>
       <c r="C57">
@@ -5133,7 +5142,7 @@
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" t="s">
         <v>1</v>
       </c>
       <c r="C58">
@@ -5144,7 +5153,7 @@
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" t="s">
         <v>1</v>
       </c>
       <c r="C59">
@@ -5155,7 +5164,7 @@
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" t="s">
         <v>1</v>
       </c>
       <c r="C60">
@@ -5166,7 +5175,7 @@
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" t="s">
         <v>1</v>
       </c>
       <c r="C61">
@@ -5177,7 +5186,7 @@
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" t="s">
         <v>1</v>
       </c>
       <c r="C62">
@@ -5188,7 +5197,7 @@
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" t="s">
         <v>1</v>
       </c>
       <c r="C63">
@@ -5199,7 +5208,7 @@
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" t="s">
         <v>1</v>
       </c>
       <c r="C64">
@@ -5210,7 +5219,7 @@
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" t="s">
         <v>1</v>
       </c>
       <c r="C65">
@@ -5221,7 +5230,7 @@
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" t="s">
         <v>1</v>
       </c>
       <c r="C66">
@@ -5232,7 +5241,7 @@
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" t="s">
         <v>1</v>
       </c>
       <c r="C67">
@@ -5243,7 +5252,7 @@
       <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" t="s">
         <v>1</v>
       </c>
       <c r="C68">
@@ -5288,7 +5297,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
@@ -5299,7 +5308,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
@@ -5310,7 +5319,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4">
@@ -5321,7 +5330,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5">
@@ -5332,7 +5341,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6">
@@ -5343,7 +5352,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7">
@@ -5354,7 +5363,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8">
@@ -5365,7 +5374,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9">
@@ -5376,7 +5385,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10">
@@ -5387,7 +5396,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="C11">
@@ -5398,7 +5407,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
       <c r="C12">
@@ -5409,7 +5418,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13">
@@ -5420,7 +5429,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14">
@@ -5431,7 +5440,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15">
@@ -5442,7 +5451,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="C16">
@@ -5453,7 +5462,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17">
@@ -5464,7 +5473,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="C18">
@@ -5475,7 +5484,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" t="s">
         <v>1</v>
       </c>
       <c r="C19">
@@ -5486,7 +5495,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="C20">
@@ -5497,7 +5506,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" t="s">
         <v>1</v>
       </c>
       <c r="C21">
@@ -5508,7 +5517,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" t="s">
         <v>1</v>
       </c>
       <c r="C22">
@@ -5519,7 +5528,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23">
@@ -5530,7 +5539,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" t="s">
         <v>1</v>
       </c>
       <c r="C24">
@@ -5541,7 +5550,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25">
@@ -5552,7 +5561,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26">
@@ -5563,7 +5572,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" t="s">
         <v>1</v>
       </c>
       <c r="C27">
@@ -5574,7 +5583,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" t="s">
         <v>1</v>
       </c>
       <c r="C28">
@@ -5585,7 +5594,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29">
@@ -5596,7 +5605,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="C30">
@@ -5607,7 +5616,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31">
@@ -5618,7 +5627,7 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" t="s">
         <v>1</v>
       </c>
       <c r="C32">
@@ -5629,7 +5638,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" t="s">
         <v>1</v>
       </c>
       <c r="C33">
@@ -5640,7 +5649,7 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34">
@@ -5651,7 +5660,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" t="s">
         <v>1</v>
       </c>
       <c r="C35">
@@ -5662,7 +5671,7 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" t="s">
         <v>1</v>
       </c>
       <c r="C36">
@@ -5673,7 +5682,7 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37">
@@ -5684,7 +5693,7 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38">
@@ -5695,7 +5704,7 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="C39">
@@ -5706,7 +5715,7 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" t="s">
         <v>1</v>
       </c>
       <c r="C40">
@@ -5717,7 +5726,7 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" t="s">
         <v>1</v>
       </c>
       <c r="C41">
@@ -5728,7 +5737,7 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" t="s">
         <v>1</v>
       </c>
       <c r="C42">
@@ -5739,7 +5748,7 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" t="s">
         <v>1</v>
       </c>
       <c r="C43">
@@ -5750,7 +5759,7 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="C44">
@@ -5761,7 +5770,7 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" t="s">
         <v>1</v>
       </c>
       <c r="C45">
@@ -5772,7 +5781,7 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" t="s">
         <v>1</v>
       </c>
       <c r="C46">
@@ -5783,7 +5792,7 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" t="s">
         <v>1</v>
       </c>
       <c r="C47">
@@ -5794,7 +5803,7 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" t="s">
         <v>1</v>
       </c>
       <c r="C48">
@@ -5805,7 +5814,7 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" t="s">
         <v>1</v>
       </c>
       <c r="C49">
@@ -5816,7 +5825,7 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" t="s">
         <v>1</v>
       </c>
       <c r="C50">
@@ -5827,7 +5836,7 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" t="s">
         <v>1</v>
       </c>
       <c r="C51">
@@ -5838,7 +5847,7 @@
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" t="s">
         <v>1</v>
       </c>
       <c r="C52">
@@ -5849,7 +5858,7 @@
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" t="s">
         <v>1</v>
       </c>
       <c r="C53">
@@ -5860,7 +5869,7 @@
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" t="s">
         <v>1</v>
       </c>
       <c r="C54">
@@ -5871,7 +5880,7 @@
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" t="s">
         <v>1</v>
       </c>
       <c r="C55">
@@ -5882,7 +5891,7 @@
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" t="s">
         <v>1</v>
       </c>
       <c r="C56">
@@ -5893,7 +5902,7 @@
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" t="s">
         <v>1</v>
       </c>
       <c r="C57">
@@ -5904,7 +5913,7 @@
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" t="s">
         <v>1</v>
       </c>
       <c r="C58">
@@ -5915,7 +5924,7 @@
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" t="s">
         <v>1</v>
       </c>
       <c r="C59">
@@ -5926,7 +5935,7 @@
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" t="s">
         <v>1</v>
       </c>
       <c r="C60">
@@ -5937,7 +5946,7 @@
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" t="s">
         <v>1</v>
       </c>
       <c r="C61">
@@ -5948,7 +5957,7 @@
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" t="s">
         <v>1</v>
       </c>
       <c r="C62">
@@ -5959,7 +5968,7 @@
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" t="s">
         <v>1</v>
       </c>
       <c r="C63">
@@ -5970,7 +5979,7 @@
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" t="s">
         <v>1</v>
       </c>
       <c r="C64">
@@ -5981,7 +5990,7 @@
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" t="s">
         <v>1</v>
       </c>
       <c r="C65">
@@ -5992,7 +6001,7 @@
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" t="s">
         <v>1</v>
       </c>
       <c r="C66">
@@ -6003,7 +6012,7 @@
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" t="s">
         <v>1</v>
       </c>
       <c r="C67">
@@ -6014,7 +6023,7 @@
       <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" t="s">
         <v>1</v>
       </c>
       <c r="C68">
@@ -6025,7 +6034,7 @@
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B69" t="s">
         <v>1</v>
       </c>
       <c r="C69">
@@ -6036,7 +6045,7 @@
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" t="s">
         <v>1</v>
       </c>
       <c r="C70">
@@ -6047,7 +6056,7 @@
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" t="s">
         <v>1</v>
       </c>
       <c r="C71">
@@ -6058,7 +6067,7 @@
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" t="s">
         <v>1</v>
       </c>
       <c r="C72">
@@ -6069,7 +6078,7 @@
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" t="s">
         <v>1</v>
       </c>
       <c r="C73">
@@ -6080,7 +6089,7 @@
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" t="s">
         <v>1</v>
       </c>
       <c r="C74">
@@ -6091,7 +6100,7 @@
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" t="s">
         <v>1</v>
       </c>
       <c r="C75">
@@ -6102,7 +6111,7 @@
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" t="s">
         <v>1</v>
       </c>
       <c r="C76">
@@ -6113,7 +6122,7 @@
       <c r="A77">
         <v>76</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" t="s">
         <v>1</v>
       </c>
       <c r="C77">
@@ -6124,7 +6133,7 @@
       <c r="A78">
         <v>77</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B78" t="s">
         <v>1</v>
       </c>
       <c r="C78">
@@ -6135,7 +6144,7 @@
       <c r="A79">
         <v>78</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" t="s">
         <v>1</v>
       </c>
       <c r="C79">
@@ -6146,7 +6155,7 @@
       <c r="A80">
         <v>79</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" t="s">
         <v>1</v>
       </c>
       <c r="C80">
@@ -6157,7 +6166,7 @@
       <c r="A81">
         <v>80</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" t="s">
         <v>1</v>
       </c>
       <c r="C81">
@@ -6168,7 +6177,7 @@
       <c r="A82">
         <v>81</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" t="s">
         <v>1</v>
       </c>
       <c r="C82">
@@ -6179,7 +6188,7 @@
       <c r="A83">
         <v>82</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" t="s">
         <v>1</v>
       </c>
       <c r="C83">
@@ -6190,7 +6199,7 @@
       <c r="A84">
         <v>83</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" t="s">
         <v>1</v>
       </c>
       <c r="C84">
@@ -6201,7 +6210,7 @@
       <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B85" t="s">
         <v>1</v>
       </c>
       <c r="C85">
@@ -6212,7 +6221,7 @@
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" t="s">
         <v>1</v>
       </c>
       <c r="C86">
@@ -6223,7 +6232,7 @@
       <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" t="s">
         <v>1</v>
       </c>
       <c r="C87">
@@ -6234,7 +6243,7 @@
       <c r="A88">
         <v>87</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" t="s">
         <v>1</v>
       </c>
       <c r="C88">
@@ -6245,7 +6254,7 @@
       <c r="A89">
         <v>88</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" t="s">
         <v>1</v>
       </c>
       <c r="C89">
@@ -6256,7 +6265,7 @@
       <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B90" t="s">
         <v>1</v>
       </c>
       <c r="C90">
@@ -6267,7 +6276,7 @@
       <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" t="s">
         <v>1</v>
       </c>
       <c r="C91">
@@ -6278,7 +6287,7 @@
       <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" t="s">
         <v>1</v>
       </c>
       <c r="C92">
@@ -6289,7 +6298,7 @@
       <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="B93" t="s">
         <v>1</v>
       </c>
       <c r="C93">
@@ -6300,7 +6309,7 @@
       <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B94" t="s">
         <v>1</v>
       </c>
       <c r="C94">
@@ -6311,7 +6320,7 @@
       <c r="A95">
         <v>94</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" t="s">
         <v>1</v>
       </c>
       <c r="C95">
@@ -6322,7 +6331,7 @@
       <c r="A96">
         <v>95</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B96" t="s">
         <v>1</v>
       </c>
       <c r="C96">
@@ -6333,7 +6342,7 @@
       <c r="A97">
         <v>96</v>
       </c>
-      <c r="B97" s="8" t="s">
+      <c r="B97" t="s">
         <v>1</v>
       </c>
       <c r="C97">
@@ -6344,7 +6353,7 @@
       <c r="A98">
         <v>97</v>
       </c>
-      <c r="B98" s="8" t="s">
+      <c r="B98" t="s">
         <v>1</v>
       </c>
       <c r="C98">
@@ -6355,7 +6364,7 @@
       <c r="A99">
         <v>98</v>
       </c>
-      <c r="B99" s="8" t="s">
+      <c r="B99" t="s">
         <v>1</v>
       </c>
       <c r="C99">
@@ -6366,7 +6375,7 @@
       <c r="A100">
         <v>99</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" t="s">
         <v>1</v>
       </c>
       <c r="C100">
@@ -6377,7 +6386,7 @@
       <c r="A101">
         <v>100</v>
       </c>
-      <c r="B101" s="8" t="s">
+      <c r="B101" t="s">
         <v>1</v>
       </c>
       <c r="C101">
@@ -6388,7 +6397,7 @@
       <c r="A102">
         <v>101</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" t="s">
         <v>1</v>
       </c>
       <c r="C102">
@@ -6399,7 +6408,7 @@
       <c r="A103">
         <v>102</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="B103" t="s">
         <v>1</v>
       </c>
       <c r="C103">
@@ -6410,7 +6419,7 @@
       <c r="A104">
         <v>103</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B104" t="s">
         <v>1</v>
       </c>
       <c r="C104">
@@ -6421,7 +6430,7 @@
       <c r="A105">
         <v>104</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="B105" t="s">
         <v>1</v>
       </c>
       <c r="C105">
@@ -6432,7 +6441,7 @@
       <c r="A106">
         <v>105</v>
       </c>
-      <c r="B106" s="8" t="s">
+      <c r="B106" t="s">
         <v>1</v>
       </c>
       <c r="C106">
@@ -6443,7 +6452,7 @@
       <c r="A107">
         <v>106</v>
       </c>
-      <c r="B107" s="8" t="s">
+      <c r="B107" t="s">
         <v>1</v>
       </c>
       <c r="C107">
@@ -6454,7 +6463,7 @@
       <c r="A108">
         <v>107</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B108" t="s">
         <v>1</v>
       </c>
       <c r="C108">
@@ -6465,7 +6474,7 @@
       <c r="A109">
         <v>108</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="B109" t="s">
         <v>1</v>
       </c>
       <c r="C109">
@@ -6476,7 +6485,7 @@
       <c r="A110">
         <v>109</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="B110" t="s">
         <v>1</v>
       </c>
       <c r="C110">
@@ -6487,7 +6496,7 @@
       <c r="A111">
         <v>110</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="B111" t="s">
         <v>1</v>
       </c>
       <c r="C111">
@@ -6498,7 +6507,7 @@
       <c r="A112">
         <v>111</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="B112" t="s">
         <v>1</v>
       </c>
       <c r="C112">
@@ -6509,7 +6518,7 @@
       <c r="A113">
         <v>112</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="B113" t="s">
         <v>1</v>
       </c>
       <c r="C113">
@@ -6520,7 +6529,7 @@
       <c r="A114">
         <v>113</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="B114" t="s">
         <v>1</v>
       </c>
       <c r="C114">
@@ -6531,7 +6540,7 @@
       <c r="A115">
         <v>114</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="B115" t="s">
         <v>1</v>
       </c>
       <c r="C115">
@@ -6542,7 +6551,7 @@
       <c r="A116">
         <v>115</v>
       </c>
-      <c r="B116" s="8" t="s">
+      <c r="B116" t="s">
         <v>1</v>
       </c>
       <c r="C116">
@@ -6553,7 +6562,7 @@
       <c r="A117">
         <v>116</v>
       </c>
-      <c r="B117" s="8" t="s">
+      <c r="B117" t="s">
         <v>1</v>
       </c>
       <c r="C117">
@@ -6564,7 +6573,7 @@
       <c r="A118">
         <v>117</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="B118" t="s">
         <v>1</v>
       </c>
       <c r="C118">
@@ -6575,7 +6584,7 @@
       <c r="A119">
         <v>118</v>
       </c>
-      <c r="B119" s="8" t="s">
+      <c r="B119" t="s">
         <v>1</v>
       </c>
       <c r="C119">
@@ -6586,7 +6595,7 @@
       <c r="A120">
         <v>119</v>
       </c>
-      <c r="B120" s="8" t="s">
+      <c r="B120" t="s">
         <v>1</v>
       </c>
       <c r="C120">
@@ -6597,7 +6606,7 @@
       <c r="A121">
         <v>120</v>
       </c>
-      <c r="B121" s="8" t="s">
+      <c r="B121" t="s">
         <v>1</v>
       </c>
       <c r="C121">
@@ -6614,15 +6623,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F209DE0-81BA-4590-B7A4-E5A5CD8A8B4C}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6635,214 +6644,235 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="3">
         <v>61</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="3">
         <v>59</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="3">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <f>AVERAGE(B2:B301)</f>
+        <v>30.041666666666668</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(C2:C301)</f>
+        <v>15.736842105263158</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(D2:D301)</f>
+        <v>16.417910447761194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>10</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>11</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>4</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>3</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>6</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>3</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <v>8</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>10</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>5</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <v>13</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>6</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>20</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>7</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="3">
         <v>21</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>7</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>27</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>9</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="3">
         <v>26</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="3">
         <v>9</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>25</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <v>26</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="3">
         <v>10</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="3">
         <v>23</v>
       </c>
     </row>
@@ -6850,13 +6880,13 @@
       <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>27</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>13</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>17</v>
       </c>
     </row>
@@ -6864,13 +6894,13 @@
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="3">
         <v>26</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="3">
         <v>13</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="3">
         <v>23</v>
       </c>
     </row>
@@ -6878,13 +6908,13 @@
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>39</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <v>12</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <v>24</v>
       </c>
     </row>
@@ -6892,13 +6922,13 @@
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="3">
         <v>27</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="3">
         <v>12</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="3">
         <v>15</v>
       </c>
     </row>
@@ -6906,13 +6936,13 @@
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>40</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="5">
         <v>12</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <v>14</v>
       </c>
     </row>
@@ -6920,13 +6950,13 @@
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="3">
         <v>27</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="3">
         <v>12</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="3">
         <v>14</v>
       </c>
     </row>
@@ -6934,13 +6964,13 @@
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>27</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>12</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="5">
         <v>12</v>
       </c>
     </row>
@@ -6948,13 +6978,13 @@
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="3">
         <v>36</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="3">
         <v>12</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="3">
         <v>13</v>
       </c>
     </row>
@@ -6962,13 +6992,13 @@
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="5">
         <v>21</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="5">
         <v>12</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <v>17</v>
       </c>
     </row>
@@ -6976,13 +7006,13 @@
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="3">
         <v>25</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="3">
         <v>11</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="3">
         <v>17</v>
       </c>
     </row>
@@ -6990,13 +7020,13 @@
       <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="5">
         <v>26</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="5">
         <v>12</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="5">
         <v>17</v>
       </c>
     </row>
@@ -7004,13 +7034,13 @@
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="3">
         <v>26</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="3">
         <v>12</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="3">
         <v>17</v>
       </c>
     </row>
@@ -7018,13 +7048,13 @@
       <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="5">
         <v>25</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <v>12</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="5">
         <v>17</v>
       </c>
     </row>
@@ -7032,13 +7062,13 @@
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="3">
         <v>26</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="3">
         <v>12</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="3">
         <v>16</v>
       </c>
     </row>
@@ -7046,13 +7076,13 @@
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="5">
         <v>25</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="5">
         <v>12</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="5">
         <v>17</v>
       </c>
     </row>
@@ -7060,13 +7090,13 @@
       <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="3">
         <v>27</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="3">
         <v>12</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="3">
         <v>17</v>
       </c>
     </row>
@@ -7074,13 +7104,13 @@
       <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="5">
         <v>38</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="5">
         <v>14</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="5">
         <v>16</v>
       </c>
     </row>
@@ -7088,13 +7118,13 @@
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="3">
         <v>27</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="3">
         <v>14</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="3">
         <v>22</v>
       </c>
     </row>
@@ -7102,13 +7132,13 @@
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="5">
         <v>27</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="5">
         <v>18</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="5">
         <v>15</v>
       </c>
     </row>
@@ -7116,13 +7146,13 @@
       <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="3">
         <v>36</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="3">
         <v>18</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="3">
         <v>16</v>
       </c>
     </row>
@@ -7130,13 +7160,13 @@
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="5">
         <v>25</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="5">
         <v>24</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="5">
         <v>15</v>
       </c>
     </row>
@@ -7144,13 +7174,13 @@
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="3">
         <v>25</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="3">
         <v>18</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="3">
         <v>15</v>
       </c>
     </row>
@@ -7158,13 +7188,13 @@
       <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="5">
         <v>26</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="5">
         <v>24</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="5">
         <v>15</v>
       </c>
     </row>
@@ -7172,13 +7202,13 @@
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="3">
         <v>27</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="3">
         <v>24</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="3">
         <v>13</v>
       </c>
     </row>
@@ -7186,13 +7216,13 @@
       <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="5">
         <v>38</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="5">
         <v>24</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="5">
         <v>16</v>
       </c>
     </row>
@@ -7200,13 +7230,13 @@
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="3">
         <v>27</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="3">
         <v>24</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="3">
         <v>16</v>
       </c>
     </row>
@@ -7214,13 +7244,13 @@
       <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="5">
         <v>38</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="5">
         <v>24</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="5">
         <v>13</v>
       </c>
     </row>
@@ -7228,13 +7258,13 @@
       <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="3">
         <v>27</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="3">
         <v>17</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="3">
         <v>12</v>
       </c>
     </row>
@@ -7242,13 +7272,13 @@
       <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="5">
         <v>26</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="5">
         <v>24</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="5">
         <v>13</v>
       </c>
     </row>
@@ -7256,13 +7286,13 @@
       <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="3">
         <v>25</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="3">
         <v>24</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="3">
         <v>12</v>
       </c>
     </row>
@@ -7270,13 +7300,13 @@
       <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="5">
         <v>35</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="5">
         <v>24</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="5">
         <v>13</v>
       </c>
     </row>
@@ -7284,13 +7314,13 @@
       <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="3">
         <v>26</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="3">
         <v>17</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="3">
         <v>13</v>
       </c>
     </row>
@@ -7298,13 +7328,13 @@
       <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="5">
         <v>25</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="5">
         <v>24</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="5">
         <v>16</v>
       </c>
     </row>
@@ -7312,13 +7342,13 @@
       <c r="A50" s="2">
         <v>49</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="3">
         <v>26</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="3">
         <v>24</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="3">
         <v>16</v>
       </c>
     </row>
@@ -7326,13 +7356,13 @@
       <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="5">
         <v>25</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="5">
         <v>24</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="5">
         <v>16</v>
       </c>
     </row>
@@ -7340,13 +7370,13 @@
       <c r="A52" s="2">
         <v>51</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="3">
         <v>26</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="3">
         <v>24</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="3">
         <v>16</v>
       </c>
     </row>
@@ -7354,13 +7384,13 @@
       <c r="A53" s="4">
         <v>52</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="5">
         <v>35</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="5">
         <v>24</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="5">
         <v>13</v>
       </c>
     </row>
@@ -7368,13 +7398,13 @@
       <c r="A54" s="2">
         <v>53</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="3">
         <v>26</v>
       </c>
-      <c r="C54" s="6">
+      <c r="C54" s="3">
         <v>22</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="3">
         <v>16</v>
       </c>
     </row>
@@ -7382,13 +7412,13 @@
       <c r="A55" s="4">
         <v>54</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="5">
         <v>26</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="5">
         <v>18</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D55" s="5">
         <v>16</v>
       </c>
     </row>
@@ -7396,13 +7426,13 @@
       <c r="A56" s="2">
         <v>55</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="3">
         <v>26</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56" s="3">
         <v>24</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="3">
         <v>19</v>
       </c>
     </row>
@@ -7410,13 +7440,13 @@
       <c r="A57" s="4">
         <v>56</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="5">
         <v>39</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="5">
         <v>24</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="5">
         <v>19</v>
       </c>
     </row>
@@ -7424,13 +7454,13 @@
       <c r="A58" s="2">
         <v>57</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="3">
         <v>25</v>
       </c>
-      <c r="C58" s="6">
+      <c r="C58" s="3">
         <v>18</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D58" s="3">
         <v>17</v>
       </c>
     </row>
@@ -7438,11 +7468,11 @@
       <c r="A59" s="4">
         <v>58</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="5">
         <v>26</v>
       </c>
       <c r="C59" s="5"/>
-      <c r="D59" s="7">
+      <c r="D59" s="5">
         <v>24</v>
       </c>
     </row>
@@ -7450,11 +7480,11 @@
       <c r="A60" s="2">
         <v>59</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="3">
         <v>26</v>
       </c>
       <c r="C60" s="3"/>
-      <c r="D60" s="6">
+      <c r="D60" s="3">
         <v>24</v>
       </c>
     </row>
@@ -7462,11 +7492,11 @@
       <c r="A61" s="4">
         <v>60</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="5">
         <v>38</v>
       </c>
       <c r="C61" s="5"/>
-      <c r="D61" s="7">
+      <c r="D61" s="5">
         <v>22</v>
       </c>
     </row>
@@ -7474,11 +7504,11 @@
       <c r="A62" s="2">
         <v>61</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="3">
         <v>27</v>
       </c>
       <c r="C62" s="3"/>
-      <c r="D62" s="6">
+      <c r="D62" s="3">
         <v>18</v>
       </c>
     </row>
@@ -7486,11 +7516,11 @@
       <c r="A63" s="4">
         <v>62</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="5">
         <v>26</v>
       </c>
       <c r="C63" s="5"/>
-      <c r="D63" s="7">
+      <c r="D63" s="5">
         <v>24</v>
       </c>
     </row>
@@ -7498,11 +7528,11 @@
       <c r="A64" s="2">
         <v>63</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="3">
         <v>37</v>
       </c>
       <c r="C64" s="3"/>
-      <c r="D64" s="6">
+      <c r="D64" s="3">
         <v>24</v>
       </c>
     </row>
@@ -7510,11 +7540,11 @@
       <c r="A65" s="4">
         <v>64</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" s="5">
         <v>25</v>
       </c>
       <c r="C65" s="5"/>
-      <c r="D65" s="7">
+      <c r="D65" s="5">
         <v>24</v>
       </c>
     </row>
@@ -7522,11 +7552,11 @@
       <c r="A66" s="2">
         <v>65</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="3">
         <v>27</v>
       </c>
       <c r="C66" s="3"/>
-      <c r="D66" s="6">
+      <c r="D66" s="3">
         <v>24</v>
       </c>
     </row>
@@ -7534,11 +7564,11 @@
       <c r="A67" s="4">
         <v>66</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B67" s="5">
         <v>40</v>
       </c>
       <c r="C67" s="5"/>
-      <c r="D67" s="7">
+      <c r="D67" s="5">
         <v>18</v>
       </c>
     </row>
@@ -7546,11 +7576,11 @@
       <c r="A68" s="2">
         <v>67</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="3">
         <v>27</v>
       </c>
       <c r="C68" s="3"/>
-      <c r="D68" s="6">
+      <c r="D68" s="3">
         <v>25</v>
       </c>
     </row>
@@ -7558,7 +7588,7 @@
       <c r="A69" s="4">
         <v>68</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="5">
         <v>26</v>
       </c>
       <c r="C69" s="5"/>
@@ -7568,7 +7598,7 @@
       <c r="A70" s="2">
         <v>69</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="3">
         <v>40</v>
       </c>
       <c r="C70" s="3"/>
@@ -7578,7 +7608,7 @@
       <c r="A71" s="4">
         <v>70</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" s="5">
         <v>27</v>
       </c>
       <c r="C71" s="5"/>
@@ -7588,7 +7618,7 @@
       <c r="A72" s="2">
         <v>71</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="3">
         <v>39</v>
       </c>
       <c r="C72" s="3"/>
@@ -7598,7 +7628,7 @@
       <c r="A73" s="4">
         <v>72</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73" s="5">
         <v>27</v>
       </c>
       <c r="C73" s="5"/>
@@ -7608,7 +7638,7 @@
       <c r="A74" s="2">
         <v>73</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="3">
         <v>27</v>
       </c>
       <c r="C74" s="3"/>
@@ -7618,7 +7648,7 @@
       <c r="A75" s="4">
         <v>74</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B75" s="5">
         <v>40</v>
       </c>
       <c r="C75" s="5"/>
@@ -7628,7 +7658,7 @@
       <c r="A76" s="2">
         <v>75</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="3">
         <v>28</v>
       </c>
       <c r="C76" s="3"/>
@@ -7638,7 +7668,7 @@
       <c r="A77" s="4">
         <v>76</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="5">
         <v>38</v>
       </c>
       <c r="C77" s="5"/>
@@ -7648,7 +7678,7 @@
       <c r="A78" s="2">
         <v>77</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="3">
         <v>28</v>
       </c>
       <c r="C78" s="3"/>
@@ -7658,7 +7688,7 @@
       <c r="A79" s="4">
         <v>78</v>
       </c>
-      <c r="B79" s="7">
+      <c r="B79" s="5">
         <v>40</v>
       </c>
       <c r="C79" s="5"/>
@@ -7668,7 +7698,7 @@
       <c r="A80" s="2">
         <v>79</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="3">
         <v>28</v>
       </c>
       <c r="C80" s="3"/>
@@ -7678,7 +7708,7 @@
       <c r="A81" s="4">
         <v>80</v>
       </c>
-      <c r="B81" s="7">
+      <c r="B81" s="5">
         <v>40</v>
       </c>
       <c r="C81" s="5"/>
@@ -7688,7 +7718,7 @@
       <c r="A82" s="2">
         <v>81</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="3">
         <v>26</v>
       </c>
       <c r="C82" s="3"/>
@@ -7698,7 +7728,7 @@
       <c r="A83" s="4">
         <v>82</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B83" s="5">
         <v>36</v>
       </c>
       <c r="C83" s="5"/>
@@ -7708,7 +7738,7 @@
       <c r="A84" s="2">
         <v>83</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="3">
         <v>21</v>
       </c>
       <c r="C84" s="3"/>
@@ -7718,7 +7748,7 @@
       <c r="A85" s="4">
         <v>84</v>
       </c>
-      <c r="B85" s="7">
+      <c r="B85" s="5">
         <v>20</v>
       </c>
       <c r="C85" s="5"/>
@@ -7728,7 +7758,7 @@
       <c r="A86" s="2">
         <v>85</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="3">
         <v>17</v>
       </c>
       <c r="C86" s="3"/>
@@ -7738,7 +7768,7 @@
       <c r="A87" s="4">
         <v>86</v>
       </c>
-      <c r="B87" s="7">
+      <c r="B87" s="5">
         <v>16</v>
       </c>
       <c r="C87" s="5"/>
@@ -7748,7 +7778,7 @@
       <c r="A88" s="2">
         <v>87</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="3">
         <v>17</v>
       </c>
       <c r="C88" s="3"/>
@@ -7758,7 +7788,7 @@
       <c r="A89" s="4">
         <v>88</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B89" s="5">
         <v>28</v>
       </c>
       <c r="C89" s="5"/>
@@ -7768,7 +7798,7 @@
       <c r="A90" s="2">
         <v>89</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="3">
         <v>27</v>
       </c>
       <c r="C90" s="3"/>
@@ -7778,7 +7808,7 @@
       <c r="A91" s="4">
         <v>90</v>
       </c>
-      <c r="B91" s="7">
+      <c r="B91" s="5">
         <v>29</v>
       </c>
       <c r="C91" s="5"/>
@@ -7788,7 +7818,7 @@
       <c r="A92" s="2">
         <v>91</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="3">
         <v>29</v>
       </c>
       <c r="C92" s="3"/>
@@ -7798,7 +7828,7 @@
       <c r="A93" s="4">
         <v>92</v>
       </c>
-      <c r="B93" s="7">
+      <c r="B93" s="5">
         <v>39</v>
       </c>
       <c r="C93" s="5"/>
@@ -7808,7 +7838,7 @@
       <c r="A94" s="2">
         <v>93</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="3">
         <v>28</v>
       </c>
       <c r="C94" s="3"/>
@@ -7818,7 +7848,7 @@
       <c r="A95" s="4">
         <v>94</v>
       </c>
-      <c r="B95" s="7">
+      <c r="B95" s="5">
         <v>38</v>
       </c>
       <c r="C95" s="5"/>
@@ -7828,7 +7858,7 @@
       <c r="A96" s="2">
         <v>95</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="3">
         <v>27</v>
       </c>
       <c r="C96" s="3"/>
@@ -7838,7 +7868,7 @@
       <c r="A97" s="4">
         <v>96</v>
       </c>
-      <c r="B97" s="7">
+      <c r="B97" s="5">
         <v>41</v>
       </c>
       <c r="C97" s="5"/>
@@ -7848,7 +7878,7 @@
       <c r="A98" s="2">
         <v>97</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="3">
         <v>27</v>
       </c>
       <c r="C98" s="3"/>
@@ -7858,7 +7888,7 @@
       <c r="A99" s="4">
         <v>98</v>
       </c>
-      <c r="B99" s="7">
+      <c r="B99" s="5">
         <v>40</v>
       </c>
       <c r="C99" s="5"/>
@@ -7868,7 +7898,7 @@
       <c r="A100" s="2">
         <v>99</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="3">
         <v>30</v>
       </c>
       <c r="C100" s="3"/>
@@ -7878,7 +7908,7 @@
       <c r="A101" s="4">
         <v>100</v>
       </c>
-      <c r="B101" s="7">
+      <c r="B101" s="5">
         <v>45</v>
       </c>
       <c r="C101" s="5"/>
@@ -7888,7 +7918,7 @@
       <c r="A102" s="2">
         <v>101</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B102" s="3">
         <v>45</v>
       </c>
       <c r="C102" s="3"/>
@@ -7898,7 +7928,7 @@
       <c r="A103" s="4">
         <v>102</v>
       </c>
-      <c r="B103" s="7">
+      <c r="B103" s="5">
         <v>31</v>
       </c>
       <c r="C103" s="5"/>
@@ -7908,7 +7938,7 @@
       <c r="A104" s="2">
         <v>103</v>
       </c>
-      <c r="B104" s="6">
+      <c r="B104" s="3">
         <v>44</v>
       </c>
       <c r="C104" s="3"/>
@@ -7918,7 +7948,7 @@
       <c r="A105" s="4">
         <v>104</v>
       </c>
-      <c r="B105" s="7">
+      <c r="B105" s="5">
         <v>46</v>
       </c>
       <c r="C105" s="5"/>
@@ -7928,7 +7958,7 @@
       <c r="A106" s="2">
         <v>105</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B106" s="3">
         <v>44</v>
       </c>
       <c r="C106" s="3"/>
@@ -7938,7 +7968,7 @@
       <c r="A107" s="4">
         <v>106</v>
       </c>
-      <c r="B107" s="7">
+      <c r="B107" s="5">
         <v>45</v>
       </c>
       <c r="C107" s="5"/>
@@ -7948,7 +7978,7 @@
       <c r="A108" s="2">
         <v>107</v>
       </c>
-      <c r="B108" s="6">
+      <c r="B108" s="3">
         <v>31</v>
       </c>
       <c r="C108" s="3"/>
@@ -7958,7 +7988,7 @@
       <c r="A109" s="4">
         <v>108</v>
       </c>
-      <c r="B109" s="7">
+      <c r="B109" s="5">
         <v>44</v>
       </c>
       <c r="C109" s="5"/>
@@ -7968,7 +7998,7 @@
       <c r="A110" s="2">
         <v>109</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B110" s="3">
         <v>43</v>
       </c>
       <c r="C110" s="3"/>
@@ -7978,7 +8008,7 @@
       <c r="A111" s="4">
         <v>110</v>
       </c>
-      <c r="B111" s="7">
+      <c r="B111" s="5">
         <v>44</v>
       </c>
       <c r="C111" s="5"/>
@@ -7988,7 +8018,7 @@
       <c r="A112" s="2">
         <v>111</v>
       </c>
-      <c r="B112" s="6">
+      <c r="B112" s="3">
         <v>32</v>
       </c>
       <c r="C112" s="3"/>
@@ -7998,7 +8028,7 @@
       <c r="A113" s="4">
         <v>112</v>
       </c>
-      <c r="B113" s="7">
+      <c r="B113" s="5">
         <v>45</v>
       </c>
       <c r="C113" s="5"/>
@@ -8008,7 +8038,7 @@
       <c r="A114" s="2">
         <v>113</v>
       </c>
-      <c r="B114" s="6">
+      <c r="B114" s="3">
         <v>44</v>
       </c>
       <c r="C114" s="3"/>
@@ -8018,7 +8048,7 @@
       <c r="A115" s="4">
         <v>114</v>
       </c>
-      <c r="B115" s="7">
+      <c r="B115" s="5">
         <v>46</v>
       </c>
       <c r="C115" s="5"/>
@@ -8028,7 +8058,7 @@
       <c r="A116" s="2">
         <v>115</v>
       </c>
-      <c r="B116" s="6">
+      <c r="B116" s="3">
         <v>45</v>
       </c>
       <c r="C116" s="3"/>
@@ -8038,7 +8068,7 @@
       <c r="A117" s="4">
         <v>116</v>
       </c>
-      <c r="B117" s="7">
+      <c r="B117" s="5">
         <v>31</v>
       </c>
       <c r="C117" s="5"/>
@@ -8048,7 +8078,7 @@
       <c r="A118" s="2">
         <v>117</v>
       </c>
-      <c r="B118" s="6">
+      <c r="B118" s="3">
         <v>43</v>
       </c>
       <c r="C118" s="3"/>
@@ -8058,7 +8088,7 @@
       <c r="A119" s="4">
         <v>118</v>
       </c>
-      <c r="B119" s="7">
+      <c r="B119" s="5">
         <v>46</v>
       </c>
       <c r="D119" s="5"/>
@@ -8067,7 +8097,7 @@
       <c r="A120" s="2">
         <v>119</v>
       </c>
-      <c r="B120" s="6">
+      <c r="B120" s="3">
         <v>42</v>
       </c>
       <c r="D120" s="3"/>
@@ -8076,7 +8106,7 @@
       <c r="A121" s="4">
         <v>120</v>
       </c>
-      <c r="B121" s="7">
+      <c r="B121" s="5">
         <v>41</v>
       </c>
       <c r="D121" s="5"/>

</xml_diff>